<commit_message>
Working on text. Working on castleDonjonScreen. Reorganized code and add minor fixes. Start testing.
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="castleStables" sheetId="1" r:id="rId1"/>
     <sheet name="castleBarracks" sheetId="2" r:id="rId2"/>
     <sheet name="castleCourtyard" sheetId="4" r:id="rId3"/>
+    <sheet name="donjonInsideSouth" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="62">
   <si>
     <t>First scenario</t>
   </si>
@@ -114,6 +115,99 @@
   </si>
   <si>
     <t>castleDeadBody</t>
+  </si>
+  <si>
+    <t>donjonInside</t>
+  </si>
+  <si>
+    <t>donjonCrossroads</t>
+  </si>
+  <si>
+    <t>donjonCorridorLeft</t>
+  </si>
+  <si>
+    <t>donjonDoorToAlchemist</t>
+  </si>
+  <si>
+    <t>donjonAlchemistRoomBattle</t>
+  </si>
+  <si>
+    <t>donjonAlchemistRoom</t>
+  </si>
+  <si>
+    <t>donjonAlchemistRoomDeadBody</t>
+  </si>
+  <si>
+    <t>donjonAlchemistRoomTable</t>
+  </si>
+  <si>
+    <t>donjonAlchemistRoomWorkplace</t>
+  </si>
+  <si>
+    <t>donjonDoorToDungeon</t>
+  </si>
+  <si>
+    <t>donjonDoorToWarehouse</t>
+  </si>
+  <si>
+    <t>donjonCorridorRight</t>
+  </si>
+  <si>
+    <t>donjonCorridorDeadBody</t>
+  </si>
+  <si>
+    <t>donjonDoorToMageRoom</t>
+  </si>
+  <si>
+    <t>donjonMageRoom</t>
+  </si>
+  <si>
+    <t>donjonMageRoomCommDevice</t>
+  </si>
+  <si>
+    <t>donjonMageRoomTable</t>
+  </si>
+  <si>
+    <t>donjonMageRoomSleepingPlace</t>
+  </si>
+  <si>
+    <t>donjonMageRoomPapers</t>
+  </si>
+  <si>
+    <t>donjonMageRoomReport</t>
+  </si>
+  <si>
+    <t>donjonDoorToChapel</t>
+  </si>
+  <si>
+    <t>donjonChapelBattle</t>
+  </si>
+  <si>
+    <t>donjonChapel</t>
+  </si>
+  <si>
+    <t>donjonChapelDeadKnight</t>
+  </si>
+  <si>
+    <t>donjonChapelDeadKnightHands</t>
+  </si>
+  <si>
+    <t>donjonChapelDeadKnightLegs</t>
+  </si>
+  <si>
+    <t>donjonChapelAltar</t>
+  </si>
+  <si>
+    <t>donjonChapelAltarDeadBody</t>
+  </si>
+  <si>
+    <t>donjonChapelAltarDeadBodyNote</t>
+  </si>
+  <si>
+    <t>donjonChapelPileOfCorpses</t>
+  </si>
+  <si>
+    <t>nextCorridor</t>
   </si>
 </sst>
 </file>
@@ -446,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -550,6 +644,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1685,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2341,4 +2441,758 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="42"/>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on castleDonjonScreen. Reorganized code and add minor fixes. Continuing testing.
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="castleStables" sheetId="1" r:id="rId1"/>
     <sheet name="castleBarracks" sheetId="2" r:id="rId2"/>
     <sheet name="castleCourtyard" sheetId="4" r:id="rId3"/>
     <sheet name="donjonInsideSouth" sheetId="5" r:id="rId4"/>
+    <sheet name="donjonInsideNorth" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="80">
   <si>
     <t>First scenario</t>
   </si>
@@ -208,6 +209,60 @@
   </si>
   <si>
     <t>nextCorridor</t>
+  </si>
+  <si>
+    <t>corridorToCentralHall</t>
+  </si>
+  <si>
+    <t>firstUpstairs</t>
+  </si>
+  <si>
+    <t>doorToCentralHall</t>
+  </si>
+  <si>
+    <t>corridorToWarehouse</t>
+  </si>
+  <si>
+    <t>secondDoorToWarehouse</t>
+  </si>
+  <si>
+    <t>warehouseBattle</t>
+  </si>
+  <si>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>warehouseEncounter</t>
+  </si>
+  <si>
+    <t>secondUpstairs</t>
+  </si>
+  <si>
+    <t>secondFloorPrisoner</t>
+  </si>
+  <si>
+    <t>prisonerWhoAreYou</t>
+  </si>
+  <si>
+    <t>prisonerWhatHappend</t>
+  </si>
+  <si>
+    <t>prisonerWounds</t>
+  </si>
+  <si>
+    <t>prisonerNextMove</t>
+  </si>
+  <si>
+    <t>donjonCentralRoom</t>
+  </si>
+  <si>
+    <t>donjonCentralRoomWarlord</t>
+  </si>
+  <si>
+    <t>donjonCentralRoomAfterBattle</t>
+  </si>
+  <si>
+    <t>donjonCentralRoomAfterWarlordBattle</t>
   </si>
 </sst>
 </file>
@@ -540,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -647,9 +702,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -934,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2445,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2456,6 +2508,765 @@
     <col min="2" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="29.109375" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="42"/>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2472,727 +3283,480 @@
       <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2">
-        <v>6</v>
-      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>31</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>32</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>42</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>51</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="43" t="s">
-        <v>44</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>45</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>47</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>46</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>48</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>49</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>50</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>43</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="43" t="s">
-        <v>33</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>40</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>34</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="43" t="s">
-        <v>35</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="43" t="s">
-        <v>36</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="43" t="s">
-        <v>39</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="43" t="s">
-        <v>38</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="43" t="s">
-        <v>37</v>
-      </c>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>41</v>
-      </c>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="43" t="s">
-        <v>52</v>
-      </c>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="43" t="s">
-        <v>53</v>
-      </c>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="43" t="s">
-        <v>57</v>
-      </c>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="43" t="s">
-        <v>58</v>
-      </c>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="43" t="s">
-        <v>59</v>
-      </c>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="43" t="s">
-        <v>60</v>
-      </c>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="43" t="s">
-        <v>54</v>
-      </c>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="43" t="s">
-        <v>55</v>
-      </c>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="43" t="s">
-        <v>56</v>
-      </c>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>61</v>
-      </c>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delete Inventory module. Minor fixes in CSS. Add lock orientation on mobile devices  using CSS.
</commit_message>
<xml_diff>
--- a/tests/Test.xlsx
+++ b/tests/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="castleStables" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
     <t>donjonCentralRoomAfterBattle</t>
   </si>
   <si>
-    <t>donjonCentralRoomAfterWarlordBattle</t>
+    <t>centralRoomAfterSearchWarlordCorpse</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -3255,8 +3255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>